<commit_message>
Modification des boutons + test du check_act_status => ok (ca marche sans qu'on ait rien eu besoin de faire) Parasol en position ouverte au départ du match pour le protéger car sinon il va prendre cher
</commit_message>
<xml_diff>
--- a/_Hard/Recap_ports_mosfets.xlsx
+++ b/_Hard/Recap_ports_mosfets.xlsx
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>